<commit_message>
cargue datos, socios, instructores, deportes y articulos
</commit_message>
<xml_diff>
--- a/ADMINCLUB-LABORATORIO2.xlsx
+++ b/ADMINCLUB-LABORATORIO2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mel\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mel\Desktop\AdminClub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB34DB59-1AC6-4C51-B81C-4A7639923CC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F21D10-280B-4A9B-92C2-4392D9C72072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{07667100-112E-472E-8A8F-C24E02EE9302}"/>
+    <workbookView xWindow="0" yWindow="360" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{07667100-112E-472E-8A8F-C24E02EE9302}"/>
   </bookViews>
   <sheets>
     <sheet name="Socios" sheetId="1" r:id="rId1"/>
@@ -243,9 +243,6 @@
     <t>Gatorei</t>
   </si>
   <si>
-    <t>Barrita de serial</t>
-  </si>
-  <si>
     <t>Toallas</t>
   </si>
   <si>
@@ -286,6 +283,9 @@
   </si>
   <si>
     <t>Crossfit</t>
+  </si>
+  <si>
+    <t>Barrita de cereal</t>
   </si>
 </sst>
 </file>
@@ -723,6 +723,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="3" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -759,38 +783,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="6" fontId="3" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1140,31 +1140,31 @@
     </row>
     <row r="2" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="19"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="27"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="23" t="s">
+      <c r="B3" s="28"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="24"/>
-      <c r="I3" s="25"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="33"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
     </row>
@@ -1216,7 +1216,7 @@
       <c r="D5" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="18" t="s">
         <v>29</v>
       </c>
       <c r="F5" s="7">
@@ -1251,7 +1251,7 @@
       <c r="D6" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="17" t="s">
         <v>36</v>
       </c>
       <c r="F6" s="7">
@@ -1286,7 +1286,7 @@
       <c r="D7" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="E7" s="17" t="s">
         <v>37</v>
       </c>
       <c r="F7" s="7">
@@ -1321,7 +1321,7 @@
       <c r="D8" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="29" t="s">
+      <c r="E8" s="17" t="s">
         <v>40</v>
       </c>
       <c r="F8" s="7">
@@ -1356,7 +1356,7 @@
       <c r="D9" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="29" t="s">
+      <c r="E9" s="17" t="s">
         <v>43</v>
       </c>
       <c r="F9" s="7">
@@ -1391,7 +1391,7 @@
       <c r="D10" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="31" t="s">
+      <c r="E10" s="19" t="s">
         <v>46</v>
       </c>
       <c r="F10" s="10">
@@ -1445,31 +1445,31 @@
   <sheetData>
     <row r="1" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3"/>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="19"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="27"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="23" t="s">
+      <c r="B2" s="28"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="24"/>
-      <c r="I2" s="25"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="33"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
     </row>
@@ -1521,7 +1521,7 @@
       <c r="D4" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="18" t="s">
         <v>49</v>
       </c>
       <c r="F4" s="7">
@@ -1556,7 +1556,7 @@
       <c r="D5" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="17" t="s">
         <v>52</v>
       </c>
       <c r="F5" s="7">
@@ -1591,7 +1591,7 @@
       <c r="D6" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="17" t="s">
         <v>55</v>
       </c>
       <c r="F6" s="7">
@@ -1626,7 +1626,7 @@
       <c r="D7" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="E7" s="17" t="s">
         <v>49</v>
       </c>
       <c r="F7" s="7">
@@ -1661,7 +1661,7 @@
       <c r="D8" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="29" t="s">
+      <c r="E8" s="17" t="s">
         <v>60</v>
       </c>
       <c r="F8" s="7">
@@ -1696,7 +1696,7 @@
       <c r="D9" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="E9" s="31" t="s">
+      <c r="E9" s="19" t="s">
         <v>63</v>
       </c>
       <c r="F9" s="10">
@@ -1741,8 +1741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BCD84FA-A278-4704-A578-4D02FE03E20A}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1753,13 +1753,13 @@
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="28"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="36"/>
     </row>
     <row r="3" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
@@ -1839,7 +1839,7 @@
         <v>18</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="D7" s="7">
         <v>40</v>
@@ -1857,7 +1857,7 @@
         <v>19</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D8" s="7">
         <v>400</v>
@@ -1875,7 +1875,7 @@
         <v>20</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D9" s="7">
         <v>500</v>
@@ -1893,7 +1893,7 @@
         <v>21</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D10" s="10">
         <v>1000</v>
@@ -1929,29 +1929,29 @@
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="19"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="27"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="23" t="s">
+      <c r="B3" s="28"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="24"/>
-      <c r="I3" s="25"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="33"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
@@ -2490,37 +2490,37 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="34"/>
-      <c r="B1" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="19"/>
+      <c r="A1" s="38"/>
+      <c r="B1" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="27"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="35"/>
+      <c r="A2" s="39"/>
       <c r="B2" s="13"/>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
-      <c r="E2" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="33"/>
+      <c r="E2" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="21"/>
       <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>1</v>
@@ -2736,7 +2736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3253F789-82FC-4FB3-8719-F7544CA6E319}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -2748,68 +2748,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="C1" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="37" t="s">
+    </row>
+    <row r="2" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="23">
+        <v>1111</v>
+      </c>
+      <c r="B2" s="23" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="38">
-        <v>1111</v>
-      </c>
-      <c r="B2" s="38" t="s">
+      <c r="C2" s="24">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="23">
+        <v>2222</v>
+      </c>
+      <c r="B3" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="39">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="38">
-        <v>2222</v>
-      </c>
-      <c r="B3" s="38" t="s">
+      <c r="C3" s="24">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="23">
+        <v>3333</v>
+      </c>
+      <c r="B4" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="39">
+      <c r="C4" s="24">
         <v>1700</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="38">
-        <v>3333</v>
-      </c>
-      <c r="B4" s="38" t="s">
+    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="23">
+        <v>4444</v>
+      </c>
+      <c r="B5" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="39">
-        <v>1700</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="38">
-        <v>4444</v>
-      </c>
-      <c r="B5" s="38" t="s">
+      <c r="C5" s="24">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="23">
+        <v>5555</v>
+      </c>
+      <c r="B6" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="C5" s="39">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="38">
-        <v>5555</v>
-      </c>
-      <c r="B6" s="38" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" s="39">
+      <c r="C6" s="24">
         <v>2500</v>
       </c>
     </row>

</xml_diff>

<commit_message>
cargue todos los archivos e hice el backup
</commit_message>
<xml_diff>
--- a/ADMINCLUB-LABORATORIO2.xlsx
+++ b/ADMINCLUB-LABORATORIO2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mel\Desktop\AdminClub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F21D10-280B-4A9B-92C2-4392D9C72072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86EA97A5-9AC1-41CF-9916-D3CF08604549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="360" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{07667100-112E-472E-8A8F-C24E02EE9302}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{07667100-112E-472E-8A8F-C24E02EE9302}"/>
   </bookViews>
   <sheets>
     <sheet name="Socios" sheetId="1" r:id="rId1"/>
@@ -344,13 +344,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF7030A0"/>
+        <fgColor rgb="FFEFEFEF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFEFEFEF"/>
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -673,7 +673,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -717,9 +717,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -738,7 +735,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -792,6 +789,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -801,9 +805,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF99CC"/>
       <color rgb="FFFF66CC"/>
       <color rgb="FFFF7C80"/>
-      <color rgb="FFFF99CC"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1140,31 +1144,31 @@
     </row>
     <row r="2" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="27"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="26"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="31" t="s">
+      <c r="B3" s="27"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="32"/>
-      <c r="I3" s="33"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="32"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
     </row>
@@ -1216,7 +1220,7 @@
       <c r="D5" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="17" t="s">
         <v>29</v>
       </c>
       <c r="F5" s="7">
@@ -1251,7 +1255,7 @@
       <c r="D6" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="16" t="s">
         <v>36</v>
       </c>
       <c r="F6" s="7">
@@ -1286,7 +1290,7 @@
       <c r="D7" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="16" t="s">
         <v>37</v>
       </c>
       <c r="F7" s="7">
@@ -1321,7 +1325,7 @@
       <c r="D8" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="16" t="s">
         <v>40</v>
       </c>
       <c r="F8" s="7">
@@ -1356,7 +1360,7 @@
       <c r="D9" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="16" t="s">
         <v>43</v>
       </c>
       <c r="F9" s="7">
@@ -1391,7 +1395,7 @@
       <c r="D10" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="18" t="s">
         <v>46</v>
       </c>
       <c r="F10" s="10">
@@ -1445,31 +1449,31 @@
   <sheetData>
     <row r="1" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3"/>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="27"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="26"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="31" t="s">
+      <c r="B2" s="27"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="32"/>
-      <c r="I2" s="33"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="32"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
     </row>
@@ -1521,7 +1525,7 @@
       <c r="D4" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="17" t="s">
         <v>49</v>
       </c>
       <c r="F4" s="7">
@@ -1556,7 +1560,7 @@
       <c r="D5" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="16" t="s">
         <v>52</v>
       </c>
       <c r="F5" s="7">
@@ -1591,7 +1595,7 @@
       <c r="D6" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="16" t="s">
         <v>55</v>
       </c>
       <c r="F6" s="7">
@@ -1626,7 +1630,7 @@
       <c r="D7" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="16" t="s">
         <v>49</v>
       </c>
       <c r="F7" s="7">
@@ -1661,7 +1665,7 @@
       <c r="D8" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="16" t="s">
         <v>60</v>
       </c>
       <c r="F8" s="7">
@@ -1696,7 +1700,7 @@
       <c r="D9" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="18" t="s">
         <v>63</v>
       </c>
       <c r="F9" s="10">
@@ -1741,8 +1745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BCD84FA-A278-4704-A578-4D02FE03E20A}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1753,13 +1757,13 @@
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="36"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="35"/>
     </row>
     <row r="3" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
@@ -1917,8 +1921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BB6D8B4-B551-472D-96DB-5FDDD7768D99}">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5:H5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1929,29 +1933,29 @@
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="27"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="26"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="31" t="s">
+      <c r="B3" s="27"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="32"/>
-      <c r="I3" s="33"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="32"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
@@ -1986,10 +1990,10 @@
         <v>18</v>
       </c>
       <c r="D5" s="7">
-        <v>1111</v>
+        <v>11</v>
       </c>
       <c r="E5" s="7">
-        <v>145</v>
+        <v>2</v>
       </c>
       <c r="F5" s="7">
         <v>20</v>
@@ -2010,10 +2014,10 @@
         <v>20</v>
       </c>
       <c r="D6" s="7">
-        <v>1111</v>
+        <v>11</v>
       </c>
       <c r="E6" s="7">
-        <v>76</v>
+        <v>3</v>
       </c>
       <c r="F6" s="7">
         <v>20</v>
@@ -2034,10 +2038,10 @@
         <v>15</v>
       </c>
       <c r="D7" s="7">
-        <v>2222</v>
+        <v>22</v>
       </c>
       <c r="E7" s="7">
-        <v>82</v>
+        <v>1</v>
       </c>
       <c r="F7" s="7">
         <v>20</v>
@@ -2058,10 +2062,10 @@
         <v>15</v>
       </c>
       <c r="D8" s="7">
-        <v>4444</v>
+        <v>44</v>
       </c>
       <c r="E8" s="7">
-        <v>91</v>
+        <v>1</v>
       </c>
       <c r="F8" s="7">
         <v>20</v>
@@ -2082,10 +2086,10 @@
         <v>20</v>
       </c>
       <c r="D9" s="7">
-        <v>3333</v>
+        <v>33</v>
       </c>
       <c r="E9" s="7">
-        <v>112</v>
+        <v>2</v>
       </c>
       <c r="F9" s="7">
         <v>20</v>
@@ -2106,10 +2110,10 @@
         <v>19</v>
       </c>
       <c r="D10" s="7">
-        <v>1111</v>
+        <v>11</v>
       </c>
       <c r="E10" s="7">
-        <v>87</v>
+        <v>1</v>
       </c>
       <c r="F10" s="7">
         <v>20</v>
@@ -2130,10 +2134,10 @@
         <v>20</v>
       </c>
       <c r="D11" s="7">
-        <v>2222</v>
+        <v>22</v>
       </c>
       <c r="E11" s="7">
-        <v>116</v>
+        <v>1</v>
       </c>
       <c r="F11" s="7">
         <v>20</v>
@@ -2154,10 +2158,10 @@
         <v>17</v>
       </c>
       <c r="D12" s="7">
-        <v>2222</v>
+        <v>22</v>
       </c>
       <c r="E12" s="7">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="F12" s="7">
         <v>20</v>
@@ -2178,10 +2182,10 @@
         <v>21</v>
       </c>
       <c r="D13" s="7">
-        <v>1111</v>
+        <v>11</v>
       </c>
       <c r="E13" s="7">
-        <v>79</v>
+        <v>4</v>
       </c>
       <c r="F13" s="7">
         <v>20</v>
@@ -2199,13 +2203,13 @@
         <v>10</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D14" s="7">
-        <v>6666</v>
+        <v>66</v>
       </c>
       <c r="E14" s="7">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="F14" s="7">
         <v>20</v>
@@ -2217,27 +2221,27 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
-      <c r="B15" s="7">
+    <row r="15" spans="1:9" s="41" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="39"/>
+      <c r="B15" s="40">
         <v>11</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="7">
-        <v>2222</v>
-      </c>
-      <c r="E15" s="7">
-        <v>35</v>
-      </c>
-      <c r="F15" s="7">
+      <c r="C15" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="40">
+        <v>22</v>
+      </c>
+      <c r="E15" s="40">
+        <v>1</v>
+      </c>
+      <c r="F15" s="40">
         <v>20</v>
       </c>
-      <c r="G15" s="7">
-        <v>7</v>
-      </c>
-      <c r="H15" s="7">
+      <c r="G15" s="40">
+        <v>7</v>
+      </c>
+      <c r="H15" s="40">
         <v>2022</v>
       </c>
     </row>
@@ -2250,7 +2254,7 @@
         <v>21</v>
       </c>
       <c r="D16" s="7">
-        <v>3333</v>
+        <v>55</v>
       </c>
       <c r="E16" s="7">
         <v>7</v>
@@ -2274,10 +2278,10 @@
         <v>20</v>
       </c>
       <c r="D17" s="7">
-        <v>4444</v>
+        <v>44</v>
       </c>
       <c r="E17" s="7">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="F17" s="7">
         <v>20</v>
@@ -2289,27 +2293,27 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3"/>
-      <c r="B18" s="7">
+    <row r="18" spans="1:8" s="41" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="39"/>
+      <c r="B18" s="40">
         <v>14</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="7">
-        <v>1111</v>
-      </c>
-      <c r="E18" s="7">
-        <v>116</v>
-      </c>
-      <c r="F18" s="7">
+      <c r="D18" s="40">
+        <v>11</v>
+      </c>
+      <c r="E18" s="40">
+        <v>4</v>
+      </c>
+      <c r="F18" s="40">
         <v>20</v>
       </c>
-      <c r="G18" s="7">
-        <v>7</v>
-      </c>
-      <c r="H18" s="7">
+      <c r="G18" s="40">
+        <v>7</v>
+      </c>
+      <c r="H18" s="40">
         <v>2022</v>
       </c>
     </row>
@@ -2322,10 +2326,10 @@
         <v>21</v>
       </c>
       <c r="D19" s="7">
-        <v>2222</v>
+        <v>22</v>
       </c>
       <c r="E19" s="7">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="F19" s="7">
         <v>20</v>
@@ -2337,27 +2341,27 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3"/>
-      <c r="B20" s="7">
+    <row r="20" spans="1:8" s="41" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="39"/>
+      <c r="B20" s="40">
         <v>16</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="7">
-        <v>6666</v>
-      </c>
-      <c r="E20" s="7">
-        <v>9</v>
-      </c>
-      <c r="F20" s="7">
+      <c r="D20" s="40">
+        <v>66</v>
+      </c>
+      <c r="E20" s="40">
+        <v>2</v>
+      </c>
+      <c r="F20" s="40">
         <v>20</v>
       </c>
-      <c r="G20" s="7">
-        <v>7</v>
-      </c>
-      <c r="H20" s="7">
+      <c r="G20" s="40">
+        <v>7</v>
+      </c>
+      <c r="H20" s="40">
         <v>2022</v>
       </c>
     </row>
@@ -2370,10 +2374,10 @@
         <v>18</v>
       </c>
       <c r="D21" s="7">
-        <v>3333</v>
+        <v>55</v>
       </c>
       <c r="E21" s="7">
-        <v>90</v>
+        <v>3</v>
       </c>
       <c r="F21" s="7">
         <v>20</v>
@@ -2394,10 +2398,10 @@
         <v>21</v>
       </c>
       <c r="D22" s="7">
-        <v>3333</v>
+        <v>33</v>
       </c>
       <c r="E22" s="7">
-        <v>135</v>
+        <v>4</v>
       </c>
       <c r="F22" s="7">
         <v>20</v>
@@ -2409,28 +2413,28 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="3"/>
-      <c r="B23" s="15">
+    <row r="23" spans="1:8" s="41" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="39"/>
+      <c r="B23" s="40">
         <v>19</v>
       </c>
-      <c r="C23" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D23" s="15">
-        <v>1111</v>
-      </c>
-      <c r="E23" s="15">
-        <v>125</v>
-      </c>
-      <c r="F23" s="15">
+      <c r="C23" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="40">
+        <v>33</v>
+      </c>
+      <c r="E23" s="40">
+        <v>2</v>
+      </c>
+      <c r="F23" s="40">
         <v>25</v>
       </c>
-      <c r="G23" s="15">
+      <c r="G23" s="40">
         <v>12</v>
       </c>
-      <c r="H23" s="15">
-        <v>2021</v>
+      <c r="H23" s="40">
+        <v>2022</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2467,7 +2471,7 @@
       <c r="A34" s="3"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K36" s="16"/>
+      <c r="K36" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2490,32 +2494,32 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="38"/>
-      <c r="B1" s="25" t="s">
+      <c r="A1" s="37"/>
+      <c r="B1" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="27"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="26"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="39"/>
+      <c r="A2" s="38"/>
       <c r="B2" s="13"/>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
-      <c r="E2" s="37" t="s">
+      <c r="E2" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="21"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="20"/>
       <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2748,68 +2752,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="21" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23">
+      <c r="A2" s="22">
         <v>1111</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="24">
+      <c r="C2" s="23">
         <v>2500</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="23">
+      <c r="A3" s="22">
         <v>2222</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="24">
+      <c r="C3" s="23">
         <v>1700</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="23">
+      <c r="A4" s="22">
         <v>3333</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="24">
+      <c r="C4" s="23">
         <v>1700</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="23">
+      <c r="A5" s="22">
         <v>4444</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="24">
+      <c r="C5" s="23">
         <v>1000</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="23">
+      <c r="A6" s="22">
         <v>5555</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="24">
+      <c r="C6" s="23">
         <v>2500</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modificacion en el menu reportes, opcion2, problemas con diseño
</commit_message>
<xml_diff>
--- a/ADMINCLUB-LABORATORIO2.xlsx
+++ b/ADMINCLUB-LABORATORIO2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Melin\Desktop\AdminClub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA0A22DA-76FF-4F6C-985F-F4877BA80B8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD675DCF-BCFB-45A2-A055-661D3DDF2A97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6600" yWindow="3375" windowWidth="14235" windowHeight="12120" activeTab="3" xr2:uid="{07667100-112E-472E-8A8F-C24E02EE9302}"/>
+    <workbookView xWindow="0" yWindow="3375" windowWidth="14235" windowHeight="12120" activeTab="3" xr2:uid="{07667100-112E-472E-8A8F-C24E02EE9302}"/>
   </bookViews>
   <sheets>
     <sheet name="Socios" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="83">
   <si>
     <t>FECHA NACIMIENTO</t>
   </si>
@@ -286,6 +286,9 @@
   </si>
   <si>
     <t>Barrita de cereal</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> HASTA ACA SE CARGO</t>
   </si>
 </sst>
 </file>
@@ -789,6 +792,37 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -834,37 +868,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1189,8 +1192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66062287-79BB-4D31-89DC-D919ACE5E612}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:K10"/>
+    <sheetView topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1213,31 +1216,31 @@
     </row>
     <row r="2" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="29"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="40"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="33" t="s">
+      <c r="B3" s="41"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="34"/>
-      <c r="I3" s="35"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="46"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
     </row>
@@ -1518,31 +1521,31 @@
   <sheetData>
     <row r="1" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3"/>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="29"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="40"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="33" t="s">
+      <c r="B2" s="41"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="34"/>
-      <c r="I2" s="35"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="46"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
     </row>
@@ -1826,13 +1829,13 @@
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="38"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="49"/>
     </row>
     <row r="3" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
@@ -1990,8 +1993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BB6D8B4-B551-472D-96DB-5FDDD7768D99}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2002,29 +2005,29 @@
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="29"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="40"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="33" t="s">
+      <c r="B3" s="41"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="34"/>
-      <c r="I3" s="35"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="46"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
@@ -2070,7 +2073,7 @@
       <c r="G5" s="7">
         <v>7</v>
       </c>
-      <c r="H5" s="42">
+      <c r="H5" s="27">
         <v>2022</v>
       </c>
     </row>
@@ -2094,7 +2097,7 @@
       <c r="G6" s="7">
         <v>7</v>
       </c>
-      <c r="H6" s="42">
+      <c r="H6" s="27">
         <v>2022</v>
       </c>
     </row>
@@ -2118,16 +2121,13 @@
       <c r="G7" s="7">
         <v>7</v>
       </c>
-      <c r="H7" s="42">
+      <c r="H7" s="27">
         <v>2022</v>
       </c>
-      <c r="K7" s="46">
+      <c r="K7" s="31">
         <v>2018</v>
       </c>
-      <c r="L7">
-        <f>(H30+H27+H25)</f>
-        <v>6054</v>
-      </c>
+      <c r="L7" s="37"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
@@ -2149,16 +2149,13 @@
       <c r="G8" s="7">
         <v>7</v>
       </c>
-      <c r="H8" s="42">
+      <c r="H8" s="27">
         <v>2022</v>
       </c>
-      <c r="K8" s="51">
+      <c r="K8" s="36">
         <v>2019</v>
       </c>
-      <c r="L8">
-        <f>(H28+H29)</f>
-        <v>4038</v>
-      </c>
+      <c r="L8" s="37"/>
     </row>
     <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
@@ -2180,16 +2177,13 @@
       <c r="G9" s="7">
         <v>7</v>
       </c>
-      <c r="H9" s="42">
+      <c r="H9" s="27">
         <v>2022</v>
       </c>
-      <c r="K9" s="47">
+      <c r="K9" s="32">
         <v>2020</v>
       </c>
-      <c r="L9">
-        <f>(H32+H24)</f>
-        <v>4040</v>
-      </c>
+      <c r="L9" s="37"/>
     </row>
     <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
@@ -2211,16 +2205,13 @@
       <c r="G10" s="7">
         <v>7</v>
       </c>
-      <c r="H10" s="42">
+      <c r="H10" s="27">
         <v>2022</v>
       </c>
-      <c r="K10" s="49">
+      <c r="K10" s="34">
         <v>2021</v>
       </c>
-      <c r="L10">
-        <f>(H31+H26)</f>
-        <v>4042</v>
-      </c>
+      <c r="L10" s="37"/>
     </row>
     <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
@@ -2242,16 +2233,13 @@
       <c r="G11" s="7">
         <v>7</v>
       </c>
-      <c r="H11" s="42">
+      <c r="H11" s="27">
         <v>2022</v>
       </c>
-      <c r="K11" s="43">
+      <c r="K11" s="28">
         <v>2022</v>
       </c>
-      <c r="L11">
-        <f>(H5+H6+H7+H8+H9+H10+H11+H12+H13+H14+H15+H16+H17+H18+H19+H20+H21+H22+H23)</f>
-        <v>38418</v>
-      </c>
+      <c r="L11" s="37"/>
     </row>
     <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
@@ -2273,9 +2261,10 @@
       <c r="G12" s="7">
         <v>7</v>
       </c>
-      <c r="H12" s="42">
+      <c r="H12" s="27">
         <v>2022</v>
       </c>
+      <c r="L12" s="37"/>
     </row>
     <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
@@ -2297,7 +2286,7 @@
       <c r="G13" s="7">
         <v>7</v>
       </c>
-      <c r="H13" s="42">
+      <c r="H13" s="27">
         <v>2022</v>
       </c>
     </row>
@@ -2321,10 +2310,10 @@
       <c r="G14" s="7">
         <v>7</v>
       </c>
-      <c r="H14" s="42">
+      <c r="H14" s="27">
         <v>2022</v>
       </c>
-      <c r="M14" s="52"/>
+      <c r="M14" s="37"/>
     </row>
     <row r="15" spans="1:13" s="26" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="24"/>
@@ -2346,7 +2335,7 @@
       <c r="G15" s="25">
         <v>7</v>
       </c>
-      <c r="H15" s="42">
+      <c r="H15" s="27">
         <v>2022</v>
       </c>
     </row>
@@ -2370,11 +2359,12 @@
       <c r="G16" s="7">
         <v>7</v>
       </c>
-      <c r="H16" s="42">
+      <c r="H16" s="27">
         <v>2022</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L16" s="37"/>
+    </row>
+    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="7">
         <v>13</v>
@@ -2394,11 +2384,11 @@
       <c r="G17" s="7">
         <v>7</v>
       </c>
-      <c r="H17" s="42">
+      <c r="H17" s="27">
         <v>2022</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="26" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" s="26" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="24"/>
       <c r="B18" s="25">
         <v>14</v>
@@ -2418,11 +2408,11 @@
       <c r="G18" s="25">
         <v>7</v>
       </c>
-      <c r="H18" s="42">
+      <c r="H18" s="27">
         <v>2022</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="7">
         <v>15</v>
@@ -2442,11 +2432,11 @@
       <c r="G19" s="7">
         <v>7</v>
       </c>
-      <c r="H19" s="42">
+      <c r="H19" s="27">
         <v>2022</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="26" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" s="26" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="24"/>
       <c r="B20" s="25">
         <v>16</v>
@@ -2466,11 +2456,11 @@
       <c r="G20" s="25">
         <v>7</v>
       </c>
-      <c r="H20" s="42">
+      <c r="H20" s="27">
         <v>2022</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="7">
         <v>17</v>
@@ -2490,11 +2480,11 @@
       <c r="G21" s="7">
         <v>7</v>
       </c>
-      <c r="H21" s="42">
+      <c r="H21" s="27">
         <v>2022</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="7">
         <v>18</v>
@@ -2514,11 +2504,11 @@
       <c r="G22" s="7">
         <v>7</v>
       </c>
-      <c r="H22" s="42">
+      <c r="H22" s="27">
         <v>2022</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="26" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" s="26" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="24"/>
       <c r="B23" s="25">
         <v>19</v>
@@ -2538,11 +2528,11 @@
       <c r="G23" s="25">
         <v>12</v>
       </c>
-      <c r="H23" s="42">
+      <c r="H23" s="27">
         <v>2022</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="7">
         <v>20</v>
@@ -2557,16 +2547,19 @@
         <v>3</v>
       </c>
       <c r="F24" s="7">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G24" s="7">
-        <v>7</v>
-      </c>
-      <c r="H24" s="44">
+        <v>3</v>
+      </c>
+      <c r="H24" s="29">
         <v>2020</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="7">
         <v>21</v>
@@ -2586,11 +2579,11 @@
       <c r="G25" s="7">
         <v>7</v>
       </c>
-      <c r="H25" s="45">
+      <c r="H25" s="30">
         <v>2018</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="7">
         <v>22</v>
@@ -2610,11 +2603,11 @@
       <c r="G26" s="7">
         <v>7</v>
       </c>
-      <c r="H26" s="48">
+      <c r="H26" s="33">
         <v>2021</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="25">
         <v>23</v>
@@ -2634,11 +2627,11 @@
       <c r="G27" s="25">
         <v>7</v>
       </c>
-      <c r="H27" s="45">
+      <c r="H27" s="30">
         <v>2018</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="7">
         <v>24</v>
@@ -2658,11 +2651,11 @@
       <c r="G28" s="7">
         <v>7</v>
       </c>
-      <c r="H28" s="50">
+      <c r="H28" s="35">
         <v>2019</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="7">
         <v>25</v>
@@ -2682,11 +2675,11 @@
       <c r="G29" s="7">
         <v>7</v>
       </c>
-      <c r="H29" s="50">
+      <c r="H29" s="35">
         <v>2019</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="7">
         <v>26</v>
@@ -2706,11 +2699,11 @@
       <c r="G30" s="7">
         <v>7</v>
       </c>
-      <c r="H30" s="45">
+      <c r="H30" s="30">
         <v>2018</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="7">
         <v>27</v>
@@ -2730,11 +2723,11 @@
       <c r="G31" s="7">
         <v>7</v>
       </c>
-      <c r="H31" s="48">
+      <c r="H31" s="33">
         <v>2021</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="7">
         <v>28</v>
@@ -2754,7 +2747,7 @@
       <c r="G32" s="7">
         <v>7</v>
       </c>
-      <c r="H32" s="44">
+      <c r="H32" s="29">
         <v>2020</v>
       </c>
     </row>
@@ -2789,30 +2782,30 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="40"/>
-      <c r="B1" s="27" t="s">
+      <c r="A1" s="51"/>
+      <c r="B1" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="29"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="40"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="41"/>
+      <c r="A2" s="52"/>
       <c r="B2" s="13"/>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
-      <c r="E2" s="39" t="s">
+      <c r="E2" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
       <c r="H2" s="19"/>
       <c r="I2" s="20"/>
       <c r="J2" s="4"/>

</xml_diff>

<commit_message>
elimine la opcion de reportes y modifique unas cositas de dissño a mano. arregle unas cositas al mostrar los socios
</commit_message>
<xml_diff>
--- a/ADMINCLUB-LABORATORIO2.xlsx
+++ b/ADMINCLUB-LABORATORIO2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Melin\Desktop\AdminClub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD675DCF-BCFB-45A2-A055-661D3DDF2A97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F66CB606-CA39-4638-BC46-539F439E67E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3375" windowWidth="14235" windowHeight="12120" activeTab="3" xr2:uid="{07667100-112E-472E-8A8F-C24E02EE9302}"/>
+    <workbookView xWindow="0" yWindow="4080" windowWidth="14235" windowHeight="12120" xr2:uid="{07667100-112E-472E-8A8F-C24E02EE9302}"/>
   </bookViews>
   <sheets>
     <sheet name="Socios" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="88">
   <si>
     <t>FECHA NACIMIENTO</t>
   </si>
@@ -289,6 +289,21 @@
   </si>
   <si>
     <t xml:space="preserve"> HASTA ACA SE CARGO</t>
+  </si>
+  <si>
+    <t>Marcela</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toloza </t>
+  </si>
+  <si>
+    <t>mtoloza@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> hasta aca, todos los demas estan true</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -334,7 +349,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -395,8 +410,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="24">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -709,12 +730,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -823,6 +866,16 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -866,6 +919,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1190,10 +1246,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66062287-79BB-4D31-89DC-D919ACE5E612}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5:K11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1201,7 +1257,7 @@
     <col min="5" max="5" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1214,37 +1270,37 @@
       <c r="J1" s="2"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="40"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="44"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="44" t="s">
+      <c r="B3" s="45"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="45"/>
-      <c r="I3" s="46"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="50"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
     </row>
-    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>24</v>
       </c>
@@ -1279,7 +1335,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>221</v>
       </c>
@@ -1314,7 +1370,7 @@
         <v>5555</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>222</v>
       </c>
@@ -1349,7 +1405,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>223</v>
       </c>
@@ -1384,7 +1440,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>224</v>
       </c>
@@ -1412,14 +1468,17 @@
       <c r="I8" s="7">
         <v>1995</v>
       </c>
-      <c r="J8" s="9">
+      <c r="J8" s="57">
         <v>0</v>
       </c>
       <c r="K8" s="9">
         <v>2222</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>225</v>
       </c>
@@ -1454,7 +1513,7 @@
         <v>5555</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10">
         <v>226</v>
       </c>
@@ -1489,7 +1548,40 @@
         <v>2222</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="38">
+        <v>78</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" s="40" t="s">
+        <v>85</v>
+      </c>
+      <c r="F11" s="38">
+        <v>42399378</v>
+      </c>
+      <c r="G11" s="38">
+        <v>17</v>
+      </c>
+      <c r="H11" s="38">
+        <v>1</v>
+      </c>
+      <c r="I11" s="38">
+        <v>2000</v>
+      </c>
+      <c r="J11" s="41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>87</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B2:J2"/>
@@ -1503,9 +1595,10 @@
     <hyperlink ref="E8" r:id="rId4" xr:uid="{C918B804-95CE-4856-9C92-C998D12B2F4D}"/>
     <hyperlink ref="E9" r:id="rId5" xr:uid="{8AF323E3-15FD-4F97-BB60-B57C43674A35}"/>
     <hyperlink ref="E10" r:id="rId6" xr:uid="{8B4D3F3C-DDD3-4F7B-AC24-0CD4918A11BA}"/>
+    <hyperlink ref="E11" r:id="rId7" xr:uid="{793E9B29-FFA1-4508-A1EC-C68700BCBC31}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -1521,31 +1614,31 @@
   <sheetData>
     <row r="1" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3"/>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="40"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="44"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
-      <c r="B2" s="41"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="44" t="s">
+      <c r="B2" s="45"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="45"/>
-      <c r="I2" s="46"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="50"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
     </row>
@@ -1829,13 +1922,13 @@
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="49"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="53"/>
     </row>
     <row r="3" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
@@ -1993,7 +2086,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BB6D8B4-B551-472D-96DB-5FDDD7768D99}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
@@ -2005,29 +2098,29 @@
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="40"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="44"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="44" t="s">
+      <c r="B3" s="45"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="45"/>
-      <c r="I3" s="46"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="50"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
@@ -2782,30 +2875,30 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="51"/>
-      <c r="B1" s="38" t="s">
+      <c r="A1" s="55"/>
+      <c r="B1" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="40"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="44"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="52"/>
+      <c r="A2" s="56"/>
       <c r="B2" s="13"/>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
-      <c r="E2" s="50" t="s">
+      <c r="E2" s="54" t="s">
         <v>72</v>
       </c>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
       <c r="H2" s="19"/>
       <c r="I2" s="20"/>
       <c r="J2" s="4"/>

</xml_diff>

<commit_message>
arregle problemas en diseño reportes
</commit_message>
<xml_diff>
--- a/ADMINCLUB-LABORATORIO2.xlsx
+++ b/ADMINCLUB-LABORATORIO2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Melin\Desktop\AdminClub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mel\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F66CB606-CA39-4638-BC46-539F439E67E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F8DD0FD-8016-47B3-B1FA-D3EB8CB690AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4080" windowWidth="14235" windowHeight="12120" xr2:uid="{07667100-112E-472E-8A8F-C24E02EE9302}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{07667100-112E-472E-8A8F-C24E02EE9302}"/>
   </bookViews>
   <sheets>
     <sheet name="Socios" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="88">
   <si>
     <t>FECHA NACIMIENTO</t>
   </si>
@@ -876,6 +876,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -919,9 +922,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1248,7 +1248,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66062287-79BB-4D31-89DC-D919ACE5E612}">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
@@ -1272,31 +1272,31 @@
     </row>
     <row r="2" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="45"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="48" t="s">
+      <c r="B3" s="46"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="49"/>
-      <c r="I3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="51"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
     </row>
@@ -1468,7 +1468,7 @@
       <c r="I8" s="7">
         <v>1995</v>
       </c>
-      <c r="J8" s="57">
+      <c r="J8" s="42">
         <v>0</v>
       </c>
       <c r="K8" s="9">
@@ -1614,31 +1614,31 @@
   <sheetData>
     <row r="1" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3"/>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="45"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="48" t="s">
+      <c r="B2" s="46"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="49"/>
-      <c r="I2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="51"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
     </row>
@@ -1922,13 +1922,13 @@
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="54"/>
     </row>
     <row r="3" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
@@ -2086,8 +2086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BB6D8B4-B551-472D-96DB-5FDDD7768D99}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2098,29 +2098,29 @@
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="45"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="48" t="s">
+      <c r="B3" s="46"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="49"/>
-      <c r="I3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="51"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
@@ -2667,10 +2667,10 @@
         <v>4</v>
       </c>
       <c r="F25" s="7">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="G25" s="7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H25" s="30">
         <v>2018</v>
@@ -2691,10 +2691,10 @@
         <v>2</v>
       </c>
       <c r="F26" s="7">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="G26" s="7">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H26" s="33">
         <v>2021</v>
@@ -2715,10 +2715,10 @@
         <v>1</v>
       </c>
       <c r="F27" s="25">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="G27" s="25">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H27" s="30">
         <v>2018</v>
@@ -2739,118 +2739,16 @@
         <v>7</v>
       </c>
       <c r="F28" s="7">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="G28" s="7">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="H28" s="35">
         <v>2019</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="3"/>
-      <c r="B29" s="7">
-        <v>25</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D29" s="7">
-        <v>44</v>
-      </c>
-      <c r="E29" s="7">
-        <v>1</v>
-      </c>
-      <c r="F29" s="7">
-        <v>20</v>
-      </c>
-      <c r="G29" s="7">
-        <v>7</v>
-      </c>
-      <c r="H29" s="35">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="3"/>
-      <c r="B30" s="7">
-        <v>26</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D30" s="7">
-        <v>11</v>
-      </c>
-      <c r="E30" s="7">
-        <v>2</v>
-      </c>
-      <c r="F30" s="7">
-        <v>20</v>
-      </c>
-      <c r="G30" s="7">
-        <v>7</v>
-      </c>
-      <c r="H30" s="30">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="3"/>
-      <c r="B31" s="7">
-        <v>27</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D31" s="7">
-        <v>11</v>
-      </c>
-      <c r="E31" s="7">
-        <v>3</v>
-      </c>
-      <c r="F31" s="7">
-        <v>20</v>
-      </c>
-      <c r="G31" s="7">
-        <v>7</v>
-      </c>
-      <c r="H31" s="33">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="3"/>
-      <c r="B32" s="7">
-        <v>28</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D32" s="7">
-        <v>22</v>
-      </c>
-      <c r="E32" s="7">
-        <v>1</v>
-      </c>
-      <c r="F32" s="7">
-        <v>20</v>
-      </c>
-      <c r="G32" s="7">
-        <v>7</v>
-      </c>
-      <c r="H32" s="29">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="3"/>
-    </row>
-    <row r="34" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="3"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K36" s="15"/>
     </row>
   </sheetData>
@@ -2875,30 +2773,30 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="55"/>
-      <c r="B1" s="42" t="s">
+      <c r="A1" s="56"/>
+      <c r="B1" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="45"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="56"/>
+      <c r="A2" s="57"/>
       <c r="B2" s="13"/>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
-      <c r="E2" s="54" t="s">
+      <c r="E2" s="55" t="s">
         <v>72</v>
       </c>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
       <c r="H2" s="19"/>
       <c r="I2" s="20"/>
       <c r="J2" s="4"/>
@@ -3165,7 +3063,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="22">
         <v>3333</v>
       </c>
@@ -3176,7 +3074,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="22">
         <v>4444</v>
       </c>

</xml_diff>